<commit_message>
Fixed log likelihood test to match data now nans removed
</commit_message>
<xml_diff>
--- a/data/medical_dm_posterior_prior.xlsx
+++ b/data/medical_dm_posterior_prior.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gareth\cegpy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49DB9DD-0B6F-4D7D-87A1-A0E4BB2F2051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D191D5-B4F6-4934-80FB-CC1C3453F973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="2250" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,80 +585,100 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5501.5</v>
+        <f>5491+A1</f>
+        <v>5492.5</v>
       </c>
       <c r="B23">
-        <v>5501.5</v>
+        <f>5493+B1</f>
+        <v>5494.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>800.5</v>
+        <f>798+A2</f>
+        <v>798.5</v>
       </c>
       <c r="B24">
+        <f>1000+B2</f>
         <v>1000.5</v>
       </c>
       <c r="C24">
-        <v>3700.5</v>
+        <f>3693+C2</f>
+        <v>3693.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>800.5</v>
+        <f>799+A3</f>
+        <v>799.5</v>
       </c>
       <c r="B25">
-        <v>1000.5</v>
+        <f>998+B3</f>
+        <v>998.5</v>
       </c>
       <c r="C25">
-        <v>3700.5</v>
+        <f>3696+C3</f>
+        <v>3696.5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>400.25</v>
+        <f>399+A4</f>
+        <v>399.25</v>
       </c>
       <c r="B26">
-        <v>400.25</v>
+        <f>399+B4</f>
+        <v>399.25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
+        <f>500+A5</f>
         <v>500.25</v>
       </c>
       <c r="B27">
+        <f>500+B5</f>
         <v>500.25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1850.25</v>
+        <f>1846+A6</f>
+        <v>1846.25</v>
       </c>
       <c r="B28">
-        <v>1850.25</v>
+        <f>1847+B6</f>
+        <v>1847.25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
+        <f>400+A7</f>
         <v>400.25</v>
       </c>
       <c r="B29">
-        <v>400.25</v>
+        <f>399+B7</f>
+        <v>399.25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
+        <f>500+A8</f>
         <v>500.25</v>
       </c>
       <c r="B30">
-        <v>500.25</v>
+        <f>498+B8</f>
+        <v>498.25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1850.25</v>
+        <f>1849+A9</f>
+        <v>1849.25</v>
       </c>
       <c r="B31">
-        <v>1850.25</v>
+        <f>1847+B9</f>
+        <v>1847.25</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>